<commit_message>
Update team sprint 2 report and it is almost finished.
</commit_message>
<xml_diff>
--- a/documents/Unfinished_Team_Sprint2_Report.xlsx
+++ b/documents/Unfinished_Team_Sprint2_Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yn\Desktop\CS-555\week_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6FAE09-5D6C-4862-AC8D-DFDE1B276B5A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D426B1FE-3F39-42E4-B369-57F2178FE981}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="286">
   <si>
     <t>Initials</t>
   </si>
@@ -776,12 +776,6 @@
     <t>55-74</t>
   </si>
   <si>
-    <t>us12_sp</t>
-  </si>
-  <si>
-    <t>us36_sp</t>
-  </si>
-  <si>
     <t>us_rs</t>
   </si>
   <si>
@@ -824,13 +818,7 @@
     <t>us12_parent_child_agediff_limit</t>
   </si>
   <si>
-    <t>2--45</t>
-  </si>
-  <si>
     <t>us36_ppl_died_last_30days</t>
-  </si>
-  <si>
-    <t>3--32</t>
   </si>
   <si>
     <t>divorceBeforeDeath</t>
@@ -892,6 +880,21 @@
   <si>
     <t>6--31</t>
   </si>
+  <si>
+    <t>105--136</t>
+  </si>
+  <si>
+    <t>82--98</t>
+  </si>
+  <si>
+    <t>9--25</t>
+  </si>
+  <si>
+    <t>test_us36_ppl_died_last_30days_check</t>
+  </si>
+  <si>
+    <t>9--23</t>
+  </si>
 </sst>
 </file>
 
@@ -948,7 +951,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -965,12 +968,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -993,7 +990,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1052,8 +1049,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3532,7 +3530,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29:E31"/>
+      <selection activeCell="B19" sqref="B19:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3720,19 +3718,37 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>2</v>
+      </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>2</v>
+      </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3740,32 +3756,50 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
         <v>27</v>
       </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" t="s">
-        <v>48</v>
+      <c r="E14" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3773,16 +3807,16 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3790,189 +3824,216 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" t="s">
         <v>17</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
-    </row>
     <row r="19" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <v>2</v>
+      <c r="A19">
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>3</v>
+      </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
-        <v>2</v>
+      <c r="A21">
+        <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3</v>
+      </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>3</v>
+      </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>82</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>3</v>
+      </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
-        <v>2</v>
-      </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
-        <v>2</v>
-      </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
-        <v>2</v>
-      </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4951,6 +5012,9 @@
     <row r="999" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E1000">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -9130,7 +9194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -13229,7 +13293,7 @@
   <dimension ref="A1:Q1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13389,7 +13453,7 @@
       <c r="I4" s="7">
         <v>43521</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="32" t="s">
         <v>244</v>
       </c>
       <c r="L4" s="14" t="s">
@@ -24600,17 +24664,16 @@
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1" display="us01_ny.py" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
     <hyperlink ref="O2" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="K4" r:id="rId3" display="us02_sp.ny" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="O4" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="O6" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="O8" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
-    <hyperlink ref="K10" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
-    <hyperlink ref="O10" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
-    <hyperlink ref="K12" r:id="rId9" display="us35_sp.py" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
-    <hyperlink ref="O12" r:id="rId10" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
-    <hyperlink ref="K14" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
-    <hyperlink ref="O14" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
-    <hyperlink ref="O16" r:id="rId13" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="O4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="O6" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="O8" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="K10" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="O10" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="K12" r:id="rId8" display="us35_sp.py" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="O12" r:id="rId9" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="K14" r:id="rId10" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
+    <hyperlink ref="O14" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
+    <hyperlink ref="O16" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -24621,8 +24684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8:P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24725,19 +24788,19 @@
         <v>240</v>
       </c>
       <c r="L2" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="O2" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="M2" s="29" t="s">
-        <v>252</v>
-      </c>
-      <c r="O2" s="29" t="s">
-        <v>253</v>
-      </c>
       <c r="P2" s="29" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="Q2" s="29" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -24775,19 +24838,19 @@
         <v>240</v>
       </c>
       <c r="L4" s="29" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="M4" s="29" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="O4" s="29" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="P4" s="29" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="Q4" s="29" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24820,18 +24883,23 @@
         <v>43538</v>
       </c>
       <c r="K6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L6" s="29" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M6" s="31" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="O6" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="P6" s="32"/>
+        <v>253</v>
+      </c>
+      <c r="P6" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q6" s="34" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="7" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -24863,18 +24931,23 @@
         <v>43528</v>
       </c>
       <c r="K8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="L8" s="29" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="M8" s="29" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="O8" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="P8" s="32"/>
+        <v>254</v>
+      </c>
+      <c r="P8" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="9" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -24906,22 +24979,22 @@
         <v>43535</v>
       </c>
       <c r="K10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="L10" s="29" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="M10" s="29" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="O10" s="29" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="P10" s="29" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="Q10" s="29" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24954,22 +25027,22 @@
         <v>43547</v>
       </c>
       <c r="K12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="L12" s="29" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="M12" s="29" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="O12" s="29" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="P12" s="29" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="Q12" s="29" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25005,19 +25078,19 @@
         <v>239</v>
       </c>
       <c r="L14" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="M14" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="O14" s="29" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P14" s="29" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q14" s="29" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25053,19 +25126,19 @@
         <v>239</v>
       </c>
       <c r="L16" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="M16" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="O16" s="29" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="P16" s="29" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="Q16" s="29" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26090,11 +26163,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="26" width="10.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="26" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -26126,19 +26205,152 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>180</v>
+      </c>
+    </row>
     <row r="3" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>210</v>
+      </c>
+    </row>
     <row r="5" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>180</v>
+      </c>
+    </row>
     <row r="7" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>150</v>
+      </c>
+    </row>
     <row r="9" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>70</v>
+      </c>
+      <c r="F10">
+        <v>240</v>
+      </c>
+    </row>
     <row r="11" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>120</v>
+      </c>
+    </row>
     <row r="13" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+      <c r="F14">
+        <v>180</v>
+      </c>
+    </row>
     <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28180,7 +28392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>